<commit_message>
this worked, but it was slow
</commit_message>
<xml_diff>
--- a/TestFiles.xlsx
+++ b/TestFiles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0dffa0cce4dd76ba/Code/photoBackup/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="65" documentId="8_{5F8034E1-09FF-F047-B13D-26BE07FD3F27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CAEC544B-E9DC-3349-8B5E-9C1C0649BD23}"/>
+  <xr:revisionPtr revIDLastSave="66" documentId="8_{5F8034E1-09FF-F047-B13D-26BE07FD3F27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9BB4C2D-CD10-A04E-8C5E-E92DC8DC7D0D}"/>
   <bookViews>
     <workbookView xWindow="1320" yWindow="500" windowWidth="27240" windowHeight="16440" xr2:uid="{53FA82E7-C35F-0349-8446-77A1996CBB4A}"/>
   </bookViews>
@@ -475,37 +475,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB3F621F-EE55-6C4D-AFEA-642D7C214B40}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>8</v>
       </c>
       <c r="C1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>23</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -515,17 +515,17 @@
       <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>16</v>
       </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
       <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -535,17 +535,17 @@
       <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>16</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>14</v>
       </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -555,17 +555,17 @@
       <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>16</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>14</v>
       </c>
-      <c r="F4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -575,17 +575,17 @@
       <c r="C5" t="s">
         <v>10</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>16</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>14</v>
       </c>
-      <c r="F5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -595,17 +595,17 @@
       <c r="C6" t="s">
         <v>12</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>20</v>
       </c>
-      <c r="E6" t="s">
-        <v>13</v>
-      </c>
       <c r="F6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -615,17 +615,17 @@
       <c r="C7" t="s">
         <v>10</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>20</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>14</v>
       </c>
-      <c r="F7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -635,17 +635,17 @@
       <c r="C8" t="s">
         <v>11</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>20</v>
       </c>
-      <c r="E8" t="s">
-        <v>13</v>
-      </c>
       <c r="F8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -655,17 +655,17 @@
       <c r="C9" t="s">
         <v>11</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>20</v>
       </c>
-      <c r="E9" t="s">
-        <v>13</v>
-      </c>
       <c r="F9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -675,17 +675,17 @@
       <c r="C10" t="s">
         <v>11</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>21</v>
       </c>
-      <c r="E10" t="s">
-        <v>13</v>
-      </c>
       <c r="F10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -695,17 +695,17 @@
       <c r="C11" t="s">
         <v>11</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>21</v>
       </c>
-      <c r="E11" t="s">
-        <v>13</v>
-      </c>
       <c r="F11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -715,13 +715,13 @@
       <c r="C12" t="s">
         <v>11</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>22</v>
       </c>
-      <c r="E12" t="s">
-        <v>13</v>
-      </c>
       <c r="F12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>